<commit_message>
Refactor code for clarity and improve print statements; update Excel file handling in network and simulation modules.
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/template.xlsx
+++ b/jupyter_notebooks/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/mn6461_engie_com/Documents/Dokumente/GitHub/reXplan-repo/jupyter_notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\reXplan-repo\jupyter_notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{F2F30141-5F46-4937-85BE-585446A7A649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{717391F3-F426-4378-9528-11298C874AFB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A4470C-BEB7-491A-BABE-03635E704955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" firstSheet="4" activeTab="11" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="704" activeTab="10" xr2:uid="{9ECEC293-7360-4DDE-9C10-8A2C51BA16DF}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -998,21 +998,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.77734375" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -1050,155 +1050,155 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="5"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="2"/>
     </row>
   </sheetData>
@@ -1216,27 +1216,27 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1295,19 +1295,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7CE9D1-E831-4D14-93C0-93FEACE3FE30}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>90</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1326,11 +1326,11 @@
         <v>111</v>
       </c>
       <c r="C2" s="3">
-        <v>44562</v>
+        <v>45658</v>
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1338,11 +1338,11 @@
         <v>113</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -1350,11 +1350,11 @@
         <v>111</v>
       </c>
       <c r="C4" s="3">
-        <v>44562.166666666664</v>
+        <v>45658</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>113</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1375,18 +1375,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF69C053-E8BE-41F5-B9A4-E34E9036274A}">
   <dimension ref="A1:P410"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="12" customWidth="1"/>
-    <col min="10" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>89</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1486,1230 +1486,1230 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44562</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="3"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="3"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="3"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="3"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="3"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="3"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="3"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="3"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="3"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="3"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="3"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="3"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="3"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="3"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="3"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="3"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="3"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="3"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="3"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="3"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="3"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="3"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="3"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="3"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="3"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="3"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="3"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="3"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="3"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="3"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="3"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="3"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="3"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="3"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="3"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="3"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="3"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="3"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="3"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="3"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="3"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="3"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="3"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="3"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="3"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="3"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="3"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="3"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="3"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="3"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="3"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="3"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="3"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="3"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="3"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="3"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="3"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="3"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="3"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="3"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="3"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="3"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="3"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="3"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="3"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="3"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="3"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="3"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="3"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="3"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="3"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="3"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="3"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="3"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="3"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="3"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="3"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="3"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="3"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="3"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="3"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="3"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="3"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="3"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="3"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="3"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="3"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="3"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="3"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="3"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="3"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="3"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="3"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="3"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="3"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="3"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="3"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="3"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="3"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="3"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="3"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="3"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="3"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="3"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="3"/>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="3"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="3"/>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="3"/>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="3"/>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="3"/>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="3"/>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="3"/>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="3"/>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="3"/>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="3"/>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="3"/>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="3"/>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="3"/>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="3"/>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="3"/>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="3"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="3"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="3"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="3"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="3"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="3"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="3"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="3"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="3"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="3"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="3"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="3"/>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="3"/>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="3"/>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="3"/>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="3"/>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="3"/>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="3"/>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="3"/>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" s="3"/>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="3"/>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="3"/>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="3"/>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="3"/>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="3"/>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="3"/>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="3"/>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="3"/>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="3"/>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="3"/>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="3"/>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="3"/>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="3"/>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="3"/>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="3"/>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="3"/>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="3"/>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" s="3"/>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="3"/>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="3"/>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" s="3"/>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="3"/>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="3"/>
     </row>
   </sheetData>
@@ -2725,9 +2725,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2751,18 +2751,18 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -2781,16 +2781,16 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2819,50 +2819,50 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -2879,13 +2879,13 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2939,9 +2939,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2995,9 +2995,9 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3100,9 +3100,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3141,27 +3141,27 @@
       <selection activeCell="P18" sqref="P17:P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3214,49 +3214,49 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O16" s="2"/>
     </row>
   </sheetData>
@@ -3274,9 +3274,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3318,9 +3318,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3356,9 +3356,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3406,9 +3406,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3457,9 +3457,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -3492,9 +3492,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3542,9 +3542,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3601,28 +3601,28 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3675,15 +3675,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="V4" s="2"/>
     </row>
@@ -3700,38 +3700,38 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
     <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.77734375" customWidth="1"/>
-    <col min="25" max="25" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3814,15 +3814,15 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H4" s="2"/>
     </row>
   </sheetData>
@@ -3839,9 +3839,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3898,29 +3898,29 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3979,16 +3979,16 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F5" s="2"/>
     </row>
   </sheetData>
@@ -4006,23 +4006,23 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4063,62 +4063,62 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" s="5"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
     </row>
   </sheetData>
@@ -4135,19 +4135,19 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4187,21 +4187,21 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
   </sheetData>

</xml_diff>